<commit_message>
Edit Project - Photoelectric Effect (Error Fix)
</commit_message>
<xml_diff>
--- a/Photoelectric Effect/Data.xlsx
+++ b/Photoelectric Effect/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MATLAB files\Photoelectric Effect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B524D7-CACD-4DB5-A750-17943E01D8F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C06139-9D41-49D3-B1DF-7F22CB788C5F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23234" windowHeight="9100" activeTab="1" xr2:uid="{39B52070-3C48-4BDE-84C7-AE0ED18995D1}"/>
   </bookViews>
@@ -532,7 +532,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.55"/>
@@ -736,7 +736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFDDBC7A-36C1-4C23-9AB4-CDA06845D24A}">
   <dimension ref="A1:I57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="102" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="102" workbookViewId="0">
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>

</xml_diff>